<commit_message>
begin visualizations and more cleaning
</commit_message>
<xml_diff>
--- a/notebooks/baseline_data.xlsx
+++ b/notebooks/baseline_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrmik\OneDrive\Desktop\NSS\Python\Projects\Cycling_Capstone\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01238D64-8483-48BA-BBCD-20405CCA4829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFF024D-294C-4A5B-8287-9FEC929BA828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-9240" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2205,7 +2205,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -2261,7 +2261,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2566,12 +2566,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="43.109375" customWidth="1"/>
+    <col min="3" max="3" width="46.6640625" customWidth="1"/>
     <col min="5" max="5" width="37.21875" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" customWidth="1"/>
     <col min="7" max="7" width="28.44140625" customWidth="1"/>
@@ -2583,7 +2585,7 @@
     <col min="14" max="14" width="36.77734375" customWidth="1"/>
     <col min="15" max="15" width="40.44140625" customWidth="1"/>
     <col min="16" max="16" width="46.5546875" customWidth="1"/>
-    <col min="17" max="17" width="45.44140625" customWidth="1"/>
+    <col min="17" max="17" width="50.77734375" customWidth="1"/>
     <col min="18" max="18" width="112.88671875" customWidth="1"/>
     <col min="19" max="19" width="35" customWidth="1"/>
     <col min="20" max="20" width="26.77734375" customWidth="1"/>

</xml_diff>